<commit_message>
rename images of resolution images
</commit_message>
<xml_diff>
--- a/data/manualDetection/resolution/originalFiles/kai_results_210301_EV38_1_Collagen_ITSwithAsc+Dexa+IGF+TGF_63x_z-stack_2_1024x1024.xlsx
+++ b/data/manualDetection/resolution/originalFiles/kai_results_210301_EV38_1_Collagen_ITSwithAsc+Dexa+IGF+TGF_63x_z-stack_2_1024x1024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD\Daten\Cilia\manualDetection\210301_EV38_1_Collagen_ITSwithAsc+Dexa+IGF+TGF_63x_z-stack_resolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B0D645-8B5C-491F-BCCE-CC8F12DD3BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142FD1E4-E71A-4CF8-9905-BB3BDD5BA193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D4681C3C-432B-4006-A065-1F556E10F683}"/>
   </bookViews>
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EAF1B93-8D5A-4DDF-9B98-D3A4298A3DAA}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -424,13 +424,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10.02</v>
+        <v>6.0389999999999997</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -438,13 +438,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.907</v>
+        <v>6.5</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,13 +452,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5.2190000000000003</v>
+        <v>5.4909999999999997</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,13 +466,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8.0619999999999994</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,13 +480,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>8.9600000000000009</v>
+        <v>7.601</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,10 +494,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>11.336</v>
+        <v>3.0409999999999999</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>12</v>
@@ -508,13 +508,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5.2039999999999997</v>
+        <v>7.3109999999999999</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,13 +522,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>11.102</v>
+        <v>5.1989999999999998</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -536,13 +536,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6.8949999999999996</v>
+        <v>6.9390000000000001</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -550,13 +550,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.5679999999999996</v>
+        <v>9.0879999999999992</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -564,13 +564,83 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4.8070000000000004</v>
+        <v>4.8029999999999999</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>8.2520000000000007</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
+      </c>
+      <c r="B14">
+        <v>9.5879999999999992</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>10.272</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>10.808</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>8.9359999999999999</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>